<commit_message>
more changes up to Weds 25.06.2014
Includes videos for media release and new/updated Dashboards as per Ann
Penny's descriptions.
</commit_message>
<xml_diff>
--- a/Formatted_Excel_Files/Life_Expectancy.xlsx
+++ b/Formatted_Excel_Files/Life_Expectancy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="270" windowWidth="17520" windowHeight="13200" tabRatio="721" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="270" windowWidth="17520" windowHeight="13200" tabRatio="721" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8177" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8142" uniqueCount="241">
   <si>
     <t>Region</t>
   </si>
@@ -732,9 +732,6 @@
     <t>2005-2010</t>
   </si>
   <si>
-    <t>Period</t>
-  </si>
-  <si>
     <t>Avg Life Expectancy (Male &amp; Female)</t>
   </si>
   <si>
@@ -11811,8 +11808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C133"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11822,18 +11819,18 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1" t="s">
         <v>237</v>
-      </c>
-      <c r="C1" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>224</v>
+      <c r="B2">
+        <v>1950</v>
       </c>
       <c r="C2">
         <v>41.3</v>
@@ -11843,8 +11840,8 @@
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>225</v>
+      <c r="B3">
+        <v>1955</v>
       </c>
       <c r="C3">
         <v>44.4</v>
@@ -11854,8 +11851,8 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>226</v>
+      <c r="B4">
+        <v>1960</v>
       </c>
       <c r="C4">
         <v>47.3</v>
@@ -11865,8 +11862,8 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>227</v>
+      <c r="B5">
+        <v>1965</v>
       </c>
       <c r="C5">
         <v>50.9</v>
@@ -11876,8 +11873,8 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
-        <v>228</v>
+      <c r="B6">
+        <v>1970</v>
       </c>
       <c r="C6">
         <v>53.4</v>
@@ -11887,8 +11884,8 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>229</v>
+      <c r="B7">
+        <v>1975</v>
       </c>
       <c r="C7">
         <v>56.1</v>
@@ -11898,8 +11895,8 @@
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>230</v>
+      <c r="B8">
+        <v>1980</v>
       </c>
       <c r="C8">
         <v>58.1</v>
@@ -11909,8 +11906,8 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
-        <v>232</v>
+      <c r="B9">
+        <v>1985</v>
       </c>
       <c r="C9">
         <v>59.7</v>
@@ -11920,8 +11917,8 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>233</v>
+      <c r="B10">
+        <v>1990</v>
       </c>
       <c r="C10">
         <v>60.8</v>
@@ -11931,8 +11928,8 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>234</v>
+      <c r="B11">
+        <v>1995</v>
       </c>
       <c r="C11">
         <v>62</v>
@@ -11942,8 +11939,8 @@
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" t="s">
-        <v>235</v>
+      <c r="B12">
+        <v>2000</v>
       </c>
       <c r="C12">
         <v>63.5</v>
@@ -11953,8 +11950,8 @@
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B13" t="s">
-        <v>236</v>
+      <c r="B13">
+        <v>2005</v>
       </c>
       <c r="C13">
         <v>65.2</v>
@@ -13020,8 +13017,8 @@
       <c r="A110" t="s">
         <v>120</v>
       </c>
-      <c r="B110" t="s">
-        <v>224</v>
+      <c r="B110">
+        <v>1950</v>
       </c>
       <c r="C110">
         <v>53.4</v>
@@ -13031,8 +13028,8 @@
       <c r="A111" t="s">
         <v>120</v>
       </c>
-      <c r="B111" t="s">
-        <v>225</v>
+      <c r="B111">
+        <v>1955</v>
       </c>
       <c r="C111">
         <v>55.5</v>
@@ -13053,8 +13050,8 @@
       <c r="A113" t="s">
         <v>120</v>
       </c>
-      <c r="B113" t="s">
-        <v>227</v>
+      <c r="B113">
+        <v>1965</v>
       </c>
       <c r="C113">
         <v>62</v>
@@ -13064,8 +13061,8 @@
       <c r="A114" t="s">
         <v>120</v>
       </c>
-      <c r="B114" t="s">
-        <v>228</v>
+      <c r="B114">
+        <v>1970</v>
       </c>
       <c r="C114">
         <v>64.3</v>
@@ -13075,8 +13072,8 @@
       <c r="A115" t="s">
         <v>120</v>
       </c>
-      <c r="B115" t="s">
-        <v>229</v>
+      <c r="B115">
+        <v>1975</v>
       </c>
       <c r="C115">
         <v>65.900000000000006</v>
@@ -13086,8 +13083,8 @@
       <c r="A116" t="s">
         <v>120</v>
       </c>
-      <c r="B116" t="s">
-        <v>230</v>
+      <c r="B116">
+        <v>1980</v>
       </c>
       <c r="C116">
         <v>67.099999999999994</v>
@@ -13097,8 +13094,8 @@
       <c r="A117" t="s">
         <v>120</v>
       </c>
-      <c r="B117" t="s">
-        <v>232</v>
+      <c r="B117">
+        <v>1985</v>
       </c>
       <c r="C117">
         <v>68.5</v>
@@ -13108,8 +13105,8 @@
       <c r="A118" t="s">
         <v>120</v>
       </c>
-      <c r="B118" t="s">
-        <v>233</v>
+      <c r="B118">
+        <v>1990</v>
       </c>
       <c r="C118">
         <v>69.3</v>
@@ -13119,8 +13116,8 @@
       <c r="A119" t="s">
         <v>120</v>
       </c>
-      <c r="B119" t="s">
-        <v>234</v>
+      <c r="B119">
+        <v>1995</v>
       </c>
       <c r="C119">
         <v>70.2</v>
@@ -13130,8 +13127,8 @@
       <c r="A120" t="s">
         <v>120</v>
       </c>
-      <c r="B120" t="s">
-        <v>235</v>
+      <c r="B120">
+        <v>2000</v>
       </c>
       <c r="C120">
         <v>71.7</v>
@@ -13141,8 +13138,8 @@
       <c r="A121" t="s">
         <v>120</v>
       </c>
-      <c r="B121" t="s">
-        <v>236</v>
+      <c r="B121">
+        <v>2005</v>
       </c>
       <c r="C121">
         <v>72.900000000000006</v>
@@ -13152,8 +13149,8 @@
       <c r="A122" t="s">
         <v>1</v>
       </c>
-      <c r="B122" t="s">
-        <v>224</v>
+      <c r="B122">
+        <v>1950</v>
       </c>
       <c r="C122">
         <v>46.9</v>
@@ -13163,8 +13160,8 @@
       <c r="A123" t="s">
         <v>1</v>
       </c>
-      <c r="B123" t="s">
-        <v>225</v>
+      <c r="B123">
+        <v>1955</v>
       </c>
       <c r="C123">
         <v>49.4</v>
@@ -13174,8 +13171,8 @@
       <c r="A124" t="s">
         <v>1</v>
       </c>
-      <c r="B124" t="s">
-        <v>226</v>
+      <c r="B124">
+        <v>1960</v>
       </c>
       <c r="C124">
         <v>51.1</v>
@@ -13185,8 +13182,8 @@
       <c r="A125" t="s">
         <v>1</v>
       </c>
-      <c r="B125" t="s">
-        <v>227</v>
+      <c r="B125">
+        <v>1965</v>
       </c>
       <c r="C125">
         <v>56.5</v>
@@ -13196,8 +13193,8 @@
       <c r="A126" t="s">
         <v>1</v>
       </c>
-      <c r="B126" t="s">
-        <v>228</v>
+      <c r="B126">
+        <v>1970</v>
       </c>
       <c r="C126">
         <v>58.8</v>
@@ -13207,8 +13204,8 @@
       <c r="A127" t="s">
         <v>1</v>
       </c>
-      <c r="B127" t="s">
-        <v>229</v>
+      <c r="B127">
+        <v>1975</v>
       </c>
       <c r="C127">
         <v>60.7</v>
@@ -13218,8 +13215,8 @@
       <c r="A128" t="s">
         <v>1</v>
       </c>
-      <c r="B128" t="s">
-        <v>230</v>
+      <c r="B128">
+        <v>1980</v>
       </c>
       <c r="C128">
         <v>62.4</v>
@@ -13229,8 +13226,8 @@
       <c r="A129" t="s">
         <v>1</v>
       </c>
-      <c r="B129" t="s">
-        <v>232</v>
+      <c r="B129">
+        <v>1985</v>
       </c>
       <c r="C129">
         <v>64</v>
@@ -13240,8 +13237,8 @@
       <c r="A130" t="s">
         <v>1</v>
       </c>
-      <c r="B130" t="s">
-        <v>233</v>
+      <c r="B130">
+        <v>1990</v>
       </c>
       <c r="C130">
         <v>64.8</v>
@@ -13251,8 +13248,8 @@
       <c r="A131" t="s">
         <v>1</v>
       </c>
-      <c r="B131" t="s">
-        <v>234</v>
+      <c r="B131">
+        <v>1995</v>
       </c>
       <c r="C131">
         <v>65.599999999999994</v>
@@ -13262,8 +13259,8 @@
       <c r="A132" t="s">
         <v>1</v>
       </c>
-      <c r="B132" t="s">
-        <v>235</v>
+      <c r="B132">
+        <v>2000</v>
       </c>
       <c r="C132">
         <v>67.099999999999994</v>
@@ -13273,8 +13270,8 @@
       <c r="A133" t="s">
         <v>1</v>
       </c>
-      <c r="B133" t="s">
-        <v>236</v>
+      <c r="B133">
+        <v>2005</v>
       </c>
       <c r="C133">
         <v>68.7</v>
@@ -13289,7 +13286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1313"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A1261" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -13303,10 +13300,10 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D1" t="s">
         <v>239</v>
-      </c>
-      <c r="D1" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -30174,7 +30171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1328"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -30194,10 +30191,10 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>